<commit_message>
Creation du CSV pour Script
</commit_message>
<xml_diff>
--- a/import_bulk_Users-Groupes_OU_ActiveDirectory-main/import.xlsx
+++ b/import_bulk_Users-Groupes_OU_ActiveDirectory-main/import.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nassi\Music\projetParcInfo\import_bulk_Users-Groupes_OU_ActiveDirectory-main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EBE158-7DDD-4590-A7CA-85EF6FE494BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="import" sheetId="1" r:id="rId4"/>
+    <sheet name="import" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1456,15 +1465,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -1475,36 +1485,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1694,20 +1711,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1758,7 +1778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1775,7 +1795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1792,7 +1812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1809,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1826,7 +1846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1843,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1860,7 +1880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1877,7 +1897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1894,7 +1914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1911,7 +1931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1928,7 +1948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1945,7 +1965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1962,7 +1982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1979,7 +1999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1996,7 +2016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2013,7 +2033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2030,7 +2050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -2047,7 +2067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -2064,7 +2084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -2081,7 +2101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -2098,7 +2118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -2115,7 +2135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -2132,7 +2152,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
@@ -2149,7 +2169,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -2166,7 +2186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -2183,7 +2203,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -2200,7 +2220,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -2217,7 +2237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -2234,7 +2254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -2251,7 +2271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -2268,7 +2288,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2285,7 +2305,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2302,7 +2322,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -2319,7 +2339,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -2336,7 +2356,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -2353,7 +2373,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -2370,7 +2390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
@@ -2404,7 +2424,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -2421,7 +2441,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
@@ -2438,7 +2458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
@@ -2455,7 +2475,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
@@ -2489,7 +2509,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2526,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>96</v>
       </c>
@@ -2523,7 +2543,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
@@ -2540,7 +2560,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -2557,7 +2577,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -2574,7 +2594,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -2591,7 +2611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>105</v>
       </c>
@@ -2608,7 +2628,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>107</v>
       </c>
@@ -2625,7 +2645,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>109</v>
       </c>
@@ -2642,7 +2662,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -2659,7 +2679,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
@@ -2676,7 +2696,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
@@ -2693,7 +2713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
@@ -2710,7 +2730,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
@@ -2727,7 +2747,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -2744,7 +2764,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -2761,7 +2781,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>123</v>
       </c>
@@ -2778,7 +2798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>125</v>
       </c>
@@ -2795,7 +2815,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>127</v>
       </c>
@@ -2812,7 +2832,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>129</v>
       </c>
@@ -2829,7 +2849,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>131</v>
       </c>
@@ -2846,7 +2866,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>133</v>
       </c>
@@ -2863,7 +2883,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>135</v>
       </c>
@@ -2880,7 +2900,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>137</v>
       </c>
@@ -2897,7 +2917,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>139</v>
       </c>
@@ -2914,7 +2934,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>141</v>
       </c>
@@ -2931,7 +2951,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>143</v>
       </c>
@@ -2948,7 +2968,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>145</v>
       </c>
@@ -2965,7 +2985,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>147</v>
       </c>
@@ -2982,7 +3002,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>127</v>
       </c>
@@ -2999,7 +3019,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>149</v>
       </c>
@@ -3016,7 +3036,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>151</v>
       </c>
@@ -3033,7 +3053,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>153</v>
       </c>
@@ -3050,7 +3070,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>155</v>
       </c>
@@ -3067,7 +3087,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>157</v>
       </c>
@@ -3084,7 +3104,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>159</v>
       </c>
@@ -3101,7 +3121,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>161</v>
       </c>
@@ -3118,7 +3138,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>163</v>
       </c>
@@ -3135,7 +3155,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -3152,7 +3172,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>167</v>
       </c>
@@ -3169,7 +3189,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -3186,7 +3206,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>171</v>
       </c>
@@ -3203,7 +3223,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>173</v>
       </c>
@@ -3220,7 +3240,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -3237,7 +3257,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>176</v>
       </c>
@@ -3254,7 +3274,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -3271,7 +3291,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>155</v>
       </c>
@@ -3288,7 +3308,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>181</v>
       </c>
@@ -3305,7 +3325,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>183</v>
       </c>
@@ -3322,7 +3342,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>185</v>
       </c>
@@ -3339,7 +3359,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>187</v>
       </c>
@@ -3356,7 +3376,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>189</v>
       </c>
@@ -3373,7 +3393,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>191</v>
       </c>
@@ -3390,7 +3410,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>193</v>
       </c>
@@ -3407,7 +3427,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>195</v>
       </c>
@@ -3424,7 +3444,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>116</v>
       </c>
@@ -3441,7 +3461,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>198</v>
       </c>
@@ -3458,7 +3478,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>200</v>
       </c>
@@ -3475,7 +3495,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>202</v>
       </c>
@@ -3492,7 +3512,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>89</v>
       </c>
@@ -3509,7 +3529,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>185</v>
       </c>
@@ -3526,7 +3546,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>207</v>
       </c>
@@ -3543,7 +3563,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>209</v>
       </c>
@@ -3560,7 +3580,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>211</v>
       </c>
@@ -3577,7 +3597,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>213</v>
       </c>
@@ -3594,7 +3614,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>215</v>
       </c>
@@ -3611,7 +3631,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>216</v>
       </c>
@@ -3628,7 +3648,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>218</v>
       </c>
@@ -3645,7 +3665,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>220</v>
       </c>
@@ -3662,7 +3682,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>222</v>
       </c>
@@ -3679,7 +3699,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>215</v>
       </c>
@@ -3696,7 +3716,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>225</v>
       </c>
@@ -3713,7 +3733,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>227</v>
       </c>
@@ -3730,7 +3750,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>228</v>
       </c>
@@ -3747,7 +3767,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>153</v>
       </c>
@@ -3764,7 +3784,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>231</v>
       </c>
@@ -3781,7 +3801,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>233</v>
       </c>
@@ -3798,7 +3818,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>235</v>
       </c>
@@ -3815,7 +3835,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>237</v>
       </c>
@@ -3832,7 +3852,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>239</v>
       </c>
@@ -3849,7 +3869,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>89</v>
       </c>
@@ -3866,7 +3886,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>242</v>
       </c>
@@ -3883,7 +3903,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>244</v>
       </c>
@@ -3900,7 +3920,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>245</v>
       </c>
@@ -3917,7 +3937,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>247</v>
       </c>
@@ -3934,7 +3954,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>35</v>
       </c>
@@ -3951,7 +3971,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>122</v>
       </c>
@@ -3968,7 +3988,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>151</v>
       </c>
@@ -3985,7 +4005,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>252</v>
       </c>
@@ -4002,7 +4022,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>211</v>
       </c>
@@ -4019,7 +4039,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>254</v>
       </c>
@@ -4036,7 +4056,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>256</v>
       </c>
@@ -4053,7 +4073,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>258</v>
       </c>
@@ -4070,7 +4090,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>207</v>
       </c>
@@ -4087,7 +4107,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>261</v>
       </c>
@@ -4104,7 +4124,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>263</v>
       </c>
@@ -4121,7 +4141,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>265</v>
       </c>
@@ -4138,7 +4158,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>267</v>
       </c>
@@ -4155,7 +4175,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>268</v>
       </c>
@@ -4172,7 +4192,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>270</v>
       </c>
@@ -4189,7 +4209,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>141</v>
       </c>
@@ -4206,7 +4226,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>273</v>
       </c>
@@ -4223,7 +4243,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>275</v>
       </c>
@@ -4240,7 +4260,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>41</v>
       </c>
@@ -4257,7 +4277,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>245</v>
       </c>
@@ -4274,7 +4294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>233</v>
       </c>
@@ -4291,7 +4311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>211</v>
       </c>
@@ -4308,7 +4328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>35</v>
       </c>
@@ -4325,7 +4345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>281</v>
       </c>
@@ -4342,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>258</v>
       </c>
@@ -4359,7 +4379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>285</v>
       </c>
@@ -4376,7 +4396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>55</v>
       </c>
@@ -4393,7 +4413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>288</v>
       </c>
@@ -4410,7 +4430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>289</v>
       </c>
@@ -4427,7 +4447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>109</v>
       </c>
@@ -4444,7 +4464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>218</v>
       </c>
@@ -4461,7 +4481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>292</v>
       </c>
@@ -4478,7 +4498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>294</v>
       </c>
@@ -4495,7 +4515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>295</v>
       </c>
@@ -4512,7 +4532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>195</v>
       </c>
@@ -4529,7 +4549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>231</v>
       </c>
@@ -4546,7 +4566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>297</v>
       </c>
@@ -4563,7 +4583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>298</v>
       </c>
@@ -4580,7 +4600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>300</v>
       </c>
@@ -4597,7 +4617,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>302</v>
       </c>
@@ -4614,7 +4634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>303</v>
       </c>
@@ -4631,7 +4651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>225</v>
       </c>
@@ -4648,7 +4668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>306</v>
       </c>
@@ -4665,7 +4685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>308</v>
       </c>
@@ -4682,7 +4702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>310</v>
       </c>
@@ -4699,7 +4719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>312</v>
       </c>
@@ -4716,7 +4736,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>314</v>
       </c>
@@ -4733,7 +4753,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>316</v>
       </c>
@@ -4750,7 +4770,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>318</v>
       </c>
@@ -4767,7 +4787,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>93</v>
       </c>
@@ -4784,7 +4804,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>321</v>
       </c>
@@ -4801,7 +4821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>322</v>
       </c>
@@ -4818,7 +4838,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>323</v>
       </c>
@@ -4835,7 +4855,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>325</v>
       </c>
@@ -4852,7 +4872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>157</v>
       </c>
@@ -4869,7 +4889,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>22</v>
       </c>
@@ -4886,7 +4906,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>22</v>
       </c>
@@ -4903,7 +4923,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>39</v>
       </c>
@@ -4920,7 +4940,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>211</v>
       </c>
@@ -4937,7 +4957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>332</v>
       </c>
@@ -4954,7 +4974,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>92</v>
       </c>
@@ -4971,7 +4991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>173</v>
       </c>
@@ -4988,7 +5008,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>51</v>
       </c>
@@ -5005,7 +5025,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>337</v>
       </c>
@@ -5022,7 +5042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>58</v>
       </c>
@@ -5039,7 +5059,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>340</v>
       </c>
@@ -5056,7 +5076,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>341</v>
       </c>
@@ -5073,7 +5093,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>342</v>
       </c>
@@ -5090,7 +5110,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>344</v>
       </c>
@@ -5107,7 +5127,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>345</v>
       </c>
@@ -5124,7 +5144,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>347</v>
       </c>
@@ -5141,7 +5161,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>349</v>
       </c>
@@ -5158,7 +5178,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>265</v>
       </c>
@@ -5175,7 +5195,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>351</v>
       </c>
@@ -5192,7 +5212,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>353</v>
       </c>
@@ -5209,7 +5229,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>354</v>
       </c>
@@ -5226,7 +5246,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>355</v>
       </c>
@@ -5243,7 +5263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>357</v>
       </c>
@@ -5260,7 +5280,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>358</v>
       </c>
@@ -5277,7 +5297,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>360</v>
       </c>
@@ -5294,7 +5314,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>93</v>
       </c>
@@ -5311,7 +5331,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>216</v>
       </c>
@@ -5328,7 +5348,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>357</v>
       </c>
@@ -5345,7 +5365,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>364</v>
       </c>
@@ -5362,7 +5382,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>310</v>
       </c>
@@ -5379,7 +5399,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>367</v>
       </c>
@@ -5396,7 +5416,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>325</v>
       </c>
@@ -5413,7 +5433,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>187</v>
       </c>
@@ -5430,7 +5450,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>183</v>
       </c>
@@ -5447,7 +5467,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>371</v>
       </c>
@@ -5464,7 +5484,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>114</v>
       </c>
@@ -5481,7 +5501,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>289</v>
       </c>
@@ -5498,7 +5518,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>112</v>
       </c>
@@ -5515,7 +5535,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>374</v>
       </c>
@@ -5532,7 +5552,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>376</v>
       </c>
@@ -5549,7 +5569,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>378</v>
       </c>
@@ -5566,7 +5586,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>380</v>
       </c>
@@ -5583,7 +5603,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>261</v>
       </c>
@@ -5600,7 +5620,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>163</v>
       </c>
@@ -5617,7 +5637,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>273</v>
       </c>
@@ -5634,7 +5654,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>384</v>
       </c>
@@ -5651,7 +5671,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>385</v>
       </c>
@@ -5668,7 +5688,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>49</v>
       </c>
@@ -5685,7 +5705,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>313</v>
       </c>
@@ -5702,7 +5722,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>389</v>
       </c>
@@ -5719,7 +5739,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>391</v>
       </c>
@@ -5736,7 +5756,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>392</v>
       </c>
@@ -5753,7 +5773,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>125</v>
       </c>
@@ -5770,7 +5790,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>393</v>
       </c>
@@ -5787,7 +5807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>300</v>
       </c>
@@ -5804,7 +5824,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>395</v>
       </c>
@@ -5821,7 +5841,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>380</v>
       </c>
@@ -5838,7 +5858,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
@@ -5855,7 +5875,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>397</v>
       </c>
@@ -5872,7 +5892,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>114</v>
       </c>
@@ -5889,7 +5909,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>398</v>
       </c>
@@ -5906,7 +5926,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>53</v>
       </c>
@@ -5923,7 +5943,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>400</v>
       </c>
@@ -5940,7 +5960,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>402</v>
       </c>
@@ -5957,7 +5977,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>58</v>
       </c>
@@ -5974,7 +5994,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>405</v>
       </c>
@@ -5991,7 +6011,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>407</v>
       </c>
@@ -6008,7 +6028,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>53</v>
       </c>
@@ -6025,7 +6045,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>410</v>
       </c>
@@ -6042,7 +6062,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>412</v>
       </c>
@@ -6059,7 +6079,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>413</v>
       </c>
@@ -6076,7 +6096,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>414</v>
       </c>
@@ -6093,7 +6113,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>416</v>
       </c>
@@ -6110,7 +6130,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>418</v>
       </c>
@@ -6127,7 +6147,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>420</v>
       </c>
@@ -6144,7 +6164,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>422</v>
       </c>
@@ -6161,7 +6181,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>422</v>
       </c>
@@ -6178,7 +6198,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>425</v>
       </c>
@@ -6195,7 +6215,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>427</v>
       </c>
@@ -6212,7 +6232,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>155</v>
       </c>
@@ -6229,7 +6249,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>429</v>
       </c>
@@ -6246,7 +6266,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>430</v>
       </c>
@@ -6263,7 +6283,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>432</v>
       </c>
@@ -6280,7 +6300,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>288</v>
       </c>
@@ -6297,7 +6317,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>434</v>
       </c>
@@ -6314,7 +6334,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>218</v>
       </c>
@@ -6331,7 +6351,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>437</v>
       </c>
@@ -6348,7 +6368,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>439</v>
       </c>
@@ -6365,7 +6385,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>441</v>
       </c>
@@ -6382,7 +6402,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>42</v>
       </c>
@@ -6399,7 +6419,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>289</v>
       </c>
@@ -6416,7 +6436,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>445</v>
       </c>
@@ -6433,7 +6453,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>446</v>
       </c>
@@ -6450,7 +6470,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>448</v>
       </c>
@@ -6467,7 +6487,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>450</v>
       </c>
@@ -6484,7 +6504,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>119</v>
       </c>
@@ -6501,7 +6521,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>357</v>
       </c>
@@ -6518,7 +6538,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>454</v>
       </c>
@@ -6535,7 +6555,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>455</v>
       </c>
@@ -6552,7 +6572,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>306</v>
       </c>
@@ -6569,7 +6589,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>458</v>
       </c>
@@ -6586,7 +6606,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>354</v>
       </c>
@@ -6603,7 +6623,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>461</v>
       </c>
@@ -6620,7 +6640,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>413</v>
       </c>
@@ -6637,7 +6657,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>463</v>
       </c>
@@ -6654,7 +6674,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>329</v>
       </c>
@@ -6671,7 +6691,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>306</v>
       </c>
@@ -6688,7 +6708,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>466</v>
       </c>
@@ -6705,7 +6725,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>468</v>
       </c>
@@ -6722,7 +6742,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>470</v>
       </c>
@@ -6739,7 +6759,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>472</v>
       </c>
@@ -6756,7 +6776,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>292</v>
       </c>
@@ -6773,7 +6793,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>475</v>
       </c>
@@ -6790,7 +6810,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>202</v>
       </c>
@@ -6807,7 +6827,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="301">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>478</v>
       </c>
@@ -6825,6 +6845,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>